<commit_message>
update questConditionsFile and add explanation in README
</commit_message>
<xml_diff>
--- a/Auditory Tone Detection Task/questConditionsFile.xlsx
+++ b/Auditory Tone Detection Task/questConditionsFile.xlsx
@@ -1,33 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W2032175\Documents\GitHub\Open-source-Auditory-Tone-Detection-Task\Auditory Tone Detection Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\subic.LING-NILS-W10\Desktop\Experiments\Janina_Neufeld\subic_outside_scanner_experiments\auditory_tone_detection_swe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BD5EBC-7AE8-4739-9A58-5DE788432798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F71DF4-FF88-47AE-B95D-F09E42F99889}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{39D40CD4-76BC-4DB8-8C0A-D42107145D07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -425,7 +416,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,14 +465,14 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="C2">
-        <f>0.4*B2</f>
-        <v>32</v>
+        <f>1.2*B2</f>
+        <v>18</v>
       </c>
       <c r="D2">
-        <v>0.63</v>
+        <v>0.82</v>
       </c>
       <c r="E2">
         <v>3.5</v>
@@ -490,7 +481,7 @@
         <v>0.01</v>
       </c>
       <c r="G2">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="H2">
         <v>0.01</v>

</xml_diff>